<commit_message>
Mass and charge balance for all reactions
</commit_message>
<xml_diff>
--- a/sbml/galactose/Galactose_Annotations.xlsx
+++ b/sbml/galactose/Galactose_Annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="781" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Annotations" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="289">
   <si>
     <t>SBMLId</t>
   </si>
@@ -386,6 +386,12 @@
     <t>1.1.1.21</t>
   </si>
   <si>
+    <t>37967</t>
+  </si>
+  <si>
+    <t>isVersionOf</t>
+  </si>
+  <si>
     <t>R01095</t>
   </si>
   <si>
@@ -452,9 +458,6 @@
     <t>13068</t>
   </si>
   <si>
-    <t>isVersionOf</t>
-  </si>
-  <si>
     <t>^\w+__GLY\w{0,1}$</t>
   </si>
   <si>
@@ -828,6 +831,24 @@
   </si>
   <si>
     <t>+1</t>
+  </si>
+  <si>
+    <t>^\w+__h2$</t>
+  </si>
+  <si>
+    <t>CHEBI:18276</t>
+  </si>
+  <si>
+    <t>dihydrogen</t>
+  </si>
+  <si>
+    <t>C00282</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>H2 </t>
   </si>
   <si>
     <t>^\w+__rbcM$</t>
@@ -1127,12 +1148,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G268"/>
+  <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D215" activeCellId="0" sqref="D215"/>
+      <selection pane="bottomLeft" activeCell="G262" activeCellId="0" sqref="G262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3004,11 +3025,11 @@
       <c r="C102" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D102" s="7" t="n">
-        <v>12792</v>
+      <c r="D102" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>91</v>
@@ -3025,10 +3046,10 @@
         <v>10</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>90</v>
@@ -3045,10 +3066,10 @@
         <v>10</v>
       </c>
       <c r="D104" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>76</v>
@@ -3056,7 +3077,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>96</v>
@@ -3076,7 +3097,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>96</v>
@@ -3096,7 +3117,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>96</v>
@@ -3117,7 +3138,7 @@
     <row r="108" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="109" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>71</v>
@@ -3140,7 +3161,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>71</v>
@@ -3149,7 +3170,7 @@
         <v>10</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>50</v>
@@ -3160,7 +3181,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>71</v>
@@ -3180,7 +3201,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>71</v>
@@ -3189,7 +3210,7 @@
         <v>10</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>50</v>
@@ -3200,7 +3221,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>71</v>
@@ -3209,7 +3230,7 @@
         <v>10</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>50</v>
@@ -3220,7 +3241,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>71</v>
@@ -3241,7 +3262,7 @@
     <row r="115" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="116" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B116" s="16" t="s">
         <v>71</v>
@@ -3264,7 +3285,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>71</v>
@@ -3273,7 +3294,7 @@
         <v>10</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>50</v>
@@ -3284,7 +3305,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>71</v>
@@ -3304,7 +3325,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>71</v>
@@ -3313,7 +3334,7 @@
         <v>10</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>50</v>
@@ -3324,7 +3345,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>71</v>
@@ -3333,7 +3354,7 @@
         <v>10</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>50</v>
@@ -3345,7 +3366,7 @@
     <row r="121" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="122" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="15" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B122" s="16" t="s">
         <v>71</v>
@@ -3368,7 +3389,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="15" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>71</v>
@@ -3377,7 +3398,7 @@
         <v>10</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>50</v>
@@ -3388,7 +3409,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="15" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>71</v>
@@ -3408,7 +3429,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="15" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>71</v>
@@ -3417,7 +3438,7 @@
         <v>10</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>50</v>
@@ -3429,7 +3450,7 @@
     <row r="126" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="127" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B127" s="16" t="s">
         <v>71</v>
@@ -3452,7 +3473,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>71</v>
@@ -3461,7 +3482,7 @@
         <v>10</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>50</v>
@@ -3472,7 +3493,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>71</v>
@@ -3492,7 +3513,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>71</v>
@@ -3501,7 +3522,7 @@
         <v>10</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>50</v>
@@ -3512,7 +3533,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>71</v>
@@ -3521,7 +3542,7 @@
         <v>10</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>50</v>
@@ -3533,7 +3554,7 @@
     <row r="132" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="133" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B133" s="16" t="s">
         <v>71</v>
@@ -3556,7 +3577,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>71</v>
@@ -3565,7 +3586,7 @@
         <v>10</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>50</v>
@@ -3576,7 +3597,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>71</v>
@@ -3585,7 +3606,7 @@
         <v>10</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>50</v>
@@ -3600,14 +3621,14 @@
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
       <c r="E136" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F136" s="6"/>
     </row>
     <row r="137" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="138" s="14" customFormat="true" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B138" s="16" t="s">
         <v>71</v>
@@ -3633,14 +3654,14 @@
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
       <c r="E139" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F139" s="6"/>
     </row>
     <row r="140" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="141" s="14" customFormat="true" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B141" s="16" t="s">
         <v>71</v>
@@ -3664,7 +3685,7 @@
     <row r="142" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="143" s="14" customFormat="true" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B143" s="16" t="s">
         <v>71</v>
@@ -3694,22 +3715,22 @@
     </row>
     <row r="145" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D145" s="5"/>
     </row>
     <row r="146" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>50</v>
@@ -3718,83 +3739,83 @@
         <v>13</v>
       </c>
       <c r="G146" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E147" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G147" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D149" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E149" s="6"/>
       <c r="F149" s="6"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E150" s="6"/>
       <c r="F150" s="6"/>
@@ -3802,16 +3823,16 @@
     <row r="151" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="152" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E152" s="6" t="s">
         <v>50</v>
@@ -3820,83 +3841,83 @@
         <v>13</v>
       </c>
       <c r="G152" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D153" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G153" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D154" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F154" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G154" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E155" s="6"/>
       <c r="F155" s="6"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D156" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D156" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="E156" s="6"/>
       <c r="F156" s="6"/>
@@ -3904,16 +3925,16 @@
     <row r="157" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="158" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>50</v>
@@ -3922,82 +3943,82 @@
         <v>13</v>
       </c>
       <c r="G158" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F159" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G159" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E160" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G160" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F161" s="6"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E162" s="6"/>
       <c r="F162" s="6"/>
@@ -4005,16 +4026,16 @@
     <row r="163" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="164" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E164" s="6" t="s">
         <v>50</v>
@@ -4023,83 +4044,83 @@
         <v>13</v>
       </c>
       <c r="G164" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D165" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G165" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D166" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F166" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G166" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D168" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
@@ -4107,16 +4128,16 @@
     <row r="169" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>50</v>
@@ -4125,83 +4146,83 @@
         <v>13</v>
       </c>
       <c r="G170" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D171" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F171" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G171" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D172" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F172" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G172" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E173" s="6"/>
       <c r="F173" s="6"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D174" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D174" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
@@ -4209,16 +4230,16 @@
     <row r="175" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E176" s="6" t="s">
         <v>50</v>
@@ -4227,83 +4248,83 @@
         <v>13</v>
       </c>
       <c r="G176" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D177" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E177" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F177" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G177" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D178" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G178" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E179" s="6"/>
       <c r="F179" s="6"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D180" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>
@@ -4311,16 +4332,16 @@
     <row r="181" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="182" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>50</v>
@@ -4329,80 +4350,80 @@
         <v>13</v>
       </c>
       <c r="G182" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D183" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G183" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D184" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G184" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D185" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D185" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="E185" s="6"/>
       <c r="F185" s="6"/>
     </row>
     <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D186" s="19" t="n">
         <v>-2</v>
@@ -4413,16 +4434,16 @@
     <row r="187" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>50</v>
@@ -4431,83 +4452,83 @@
         <v>13</v>
       </c>
       <c r="G188" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D189" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E189" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F189" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G189" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E190" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F190" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G190" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D192" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>
@@ -4515,16 +4536,16 @@
     <row r="193" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="194" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E194" s="6" t="s">
         <v>50</v>
@@ -4533,83 +4554,83 @@
         <v>13</v>
       </c>
       <c r="G194" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D195" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E195" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G195" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D196" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F196" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G196" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="6"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D198" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
@@ -4617,16 +4638,16 @@
     <row r="199" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E200" s="6" t="s">
         <v>50</v>
@@ -4635,80 +4656,80 @@
         <v>13</v>
       </c>
       <c r="G200" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D201" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F201" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G201" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D202" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F202" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G202" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C203" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E203" s="6"/>
       <c r="F203" s="6"/>
     </row>
     <row r="204" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="15" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D204" s="19" t="n">
         <v>-3</v>
@@ -4719,16 +4740,16 @@
     <row r="205" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="206" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E206" s="6" t="s">
         <v>50</v>
@@ -4737,83 +4758,83 @@
         <v>13</v>
       </c>
       <c r="G206" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D207" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E207" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F207" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G207" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D208" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F208" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G208" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="6"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C210" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D210" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E210" s="6"/>
       <c r="F210" s="6"/>
@@ -4821,16 +4842,16 @@
     <row r="211" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="212" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E212" s="6" t="s">
         <v>50</v>
@@ -4839,80 +4860,80 @@
         <v>13</v>
       </c>
       <c r="G212" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D213" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E213" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G213" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F214" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G214" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E215" s="6"/>
       <c r="F215" s="6"/>
     </row>
     <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D216" s="19" t="n">
         <v>-3</v>
@@ -4923,16 +4944,16 @@
     <row r="217" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="218" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D218" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E218" s="6" t="s">
         <v>50</v>
@@ -4941,83 +4962,83 @@
         <v>13</v>
       </c>
       <c r="G218" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D219" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E219" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F219" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G219" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D220" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F220" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G220" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D221" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E221" s="6"/>
       <c r="F221" s="6"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D222" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E222" s="6"/>
       <c r="F222" s="6"/>
@@ -5025,16 +5046,16 @@
     <row r="223" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="224" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D224" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E224" s="6" t="s">
         <v>50</v>
@@ -5043,80 +5064,80 @@
         <v>13</v>
       </c>
       <c r="G224" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D225" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E225" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F225" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G225" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C226" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D226" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G226" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D227" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E227" s="6"/>
       <c r="F227" s="6"/>
     </row>
     <row r="228" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D228" s="19" t="n">
         <v>-3</v>
@@ -5127,16 +5148,16 @@
     <row r="229" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="230" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D230" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E230" s="6" t="s">
         <v>50</v>
@@ -5145,80 +5166,80 @@
         <v>13</v>
       </c>
       <c r="G230" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D231" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E231" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F231" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G231" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D232" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F232" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G232" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D233" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E233" s="6"/>
       <c r="F233" s="6"/>
     </row>
     <row r="234" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D234" s="19" t="n">
         <v>-3</v>
@@ -5228,16 +5249,16 @@
     <row r="235" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="236" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C236" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E236" s="6" t="s">
         <v>50</v>
@@ -5246,80 +5267,80 @@
         <v>13</v>
       </c>
       <c r="G236" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C237" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D237" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E237" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F237" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G237" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C238" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D238" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F238" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G238" s="8" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D239" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E239" s="6"/>
       <c r="F239" s="6"/>
     </row>
     <row r="240" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D240" s="19" t="n">
         <v>-4</v>
@@ -5330,16 +5351,16 @@
     <row r="241" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="242" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C242" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D242" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E242" s="6" t="s">
         <v>50</v>
@@ -5348,83 +5369,83 @@
         <v>13</v>
       </c>
       <c r="G242" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C243" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D243" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E243" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F243" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G243" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C244" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D244" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E244" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F244" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G244" s="8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D245" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E245" s="6"/>
       <c r="F245" s="6"/>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D246" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E246" s="6"/>
       <c r="F246" s="6"/>
@@ -5432,16 +5453,16 @@
     <row r="247" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="248" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C248" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D248" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E248" s="6" t="s">
         <v>50</v>
@@ -5450,83 +5471,83 @@
         <v>13</v>
       </c>
       <c r="G248" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C249" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D249" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E249" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F249" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G249" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C250" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D250" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E250" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F250" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G250" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C251" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D251" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E251" s="6"/>
       <c r="F251" s="6"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C252" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D252" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E252" s="6"/>
       <c r="F252" s="6"/>
@@ -5534,16 +5555,16 @@
     <row r="253" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="254" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C254" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D254" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E254" s="6" t="s">
         <v>50</v>
@@ -5552,83 +5573,83 @@
         <v>13</v>
       </c>
       <c r="G254" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C255" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D255" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E255" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F255" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G255" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C256" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D256" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E256" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F256" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G256" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C257" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D257" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E257" s="6"/>
       <c r="F257" s="6"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C258" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D258" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E258" s="6"/>
       <c r="F258" s="6"/>
@@ -5636,16 +5657,16 @@
     <row r="259" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="260" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C260" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D260" s="8" t="s">
-        <v>272</v>
+        <v>153</v>
       </c>
       <c r="E260" s="6" t="s">
         <v>50</v>
@@ -5653,115 +5674,101 @@
       <c r="F260" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G260" s="8" t="s">
+      <c r="G260" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C261" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D261" s="7" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B261" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C261" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D261" s="7" t="s">
+      <c r="E261" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F261" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G261" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="E261" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F261" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G261" s="0" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C262" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D262" s="8" t="s">
+      <c r="D262" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E262" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F262" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G262" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="E262" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F262" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G262" s="0" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C263" s="6" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="D263" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E263" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F263" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G263" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+      <c r="E263" s="6"/>
+      <c r="F263" s="6"/>
+    </row>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C264" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D264" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E264" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F264" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G264" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="D264" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E264" s="6"/>
+      <c r="F264" s="6"/>
     </row>
     <row r="265" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="6" t="s">
-        <v>277</v>
+    <row r="266" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="15" t="s">
+        <v>278</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C266" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D266" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E266" s="6" t="s">
         <v>50</v>
@@ -5769,34 +5776,150 @@
       <c r="F266" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G266" s="0" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="6" t="s">
-        <v>277</v>
+      <c r="G266" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="15" t="s">
+        <v>278</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C267" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D267" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E267" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F267" s="0" t="s">
+      <c r="D267" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E267" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F267" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G267" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B268" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C268" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D268" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E268" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F268" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G268" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B269" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C269" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D269" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E269" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F269" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G269" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B270" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C270" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D270" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E270" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F270" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G270" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="271" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D272" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E272" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F272" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G272" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C273" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D273" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E273" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F273" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G267" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="268" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G273" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="274" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>